<commit_message>
major updates to marketable_tech...
</commit_message>
<xml_diff>
--- a/cv/%%marketable_tech_xp.xlsx
+++ b/cv/%%marketable_tech_xp.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>rare</t>
   </si>
@@ -25,10 +25,6 @@
   </si>
   <si>
     <t>many</t>
-  </si>
-  <si>
-    <t>my strength 
-among candidates</t>
   </si>
   <si>
     <t>low</t>
@@ -56,9 +52,6 @@
     <t>excellent</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>niche</t>
   </si>
   <si>
@@ -74,9 +67,6 @@
     <t>some</t>
   </si>
   <si>
-    <t>mkt depth below the top jobs</t>
-  </si>
-  <si>
     <t>poor</t>
   </si>
   <si>
@@ -95,18 +85,12 @@
     <t>good std skillset</t>
   </si>
   <si>
-    <t>declining</t>
-  </si>
-  <si>
     <t>mostly jargons</t>
   </si>
   <si>
     <t>diverse :(</t>
   </si>
   <si>
-    <t>diverse?</t>
-  </si>
-  <si>
     <t>Regulation-driven</t>
   </si>
   <si>
@@ -114,10 +98,6 @@
   </si>
   <si>
     <t>soft mkt data #curve building, mostly in ibanks</t>
-  </si>
-  <si>
-    <t>personal accu  
-# depth</t>
   </si>
   <si>
     <t>complexity 
@@ -127,9 +107,6 @@
     <t>drv pricing/risk analytics, mostly in ibanks</t>
   </si>
   <si>
-    <t>rare. very low</t>
-  </si>
-  <si>
     <t>not theoretical</t>
   </si>
   <si>
@@ -137,10 +114,6 @@
   </si>
   <si>
     <t xml:space="preserve">devops: compiler; make file; scripting; git; </t>
-  </si>
-  <si>
-    <t>mainstream: how many
-jobs now?</t>
   </si>
   <si>
     <t>promising</t>
@@ -150,27 +123,12 @@
 GC</t>
   </si>
   <si>
-    <t>poor. Low MV</t>
-  </si>
-  <si>
     <t>slowly catching on</t>
   </si>
   <si>
     <t>bond math</t>
   </si>
   <si>
-    <t>trade execution, mostly in ibanks</t>
-  </si>
-  <si>
-    <t>OMS #Kenny</t>
-  </si>
-  <si>
-    <t>some complexity, not theoretical</t>
-  </si>
-  <si>
-    <t>too niche</t>
-  </si>
-  <si>
     <t>unknown</t>
   </si>
   <si>
@@ -186,7 +144,62 @@
     <t>mkt data,socket…</t>
   </si>
   <si>
-    <t>math-light risk sys in big ibanks</t>
+    <t>curve building</t>
+  </si>
+  <si>
+    <t>FIX + connectivity + OMS#Kenny</t>
+  </si>
+  <si>
+    <t>reasonable</t>
+  </si>
+  <si>
+    <t>possible</t>
+  </si>
+  <si>
+    <t>good chance</t>
+  </si>
+  <si>
+    <t>accu # depth</t>
+  </si>
+  <si>
+    <t>too diverse?</t>
+  </si>
+  <si>
+    <t>FIX good</t>
+  </si>
+  <si>
+    <t>mainstream? how many
+jobs now?</t>
+  </si>
+  <si>
+    <t>theoretical</t>
+  </si>
+  <si>
+    <t>math-lite risk sys in big ibanks</t>
+  </si>
+  <si>
+    <t>3 self-study</t>
+  </si>
+  <si>
+    <t>reasonable?</t>
+  </si>
+  <si>
+    <t>poor. Lower MV</t>
+  </si>
+  <si>
+    <t>7 #bash/git</t>
+  </si>
+  <si>
+    <t>declining slightly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mkt depth </t>
+  </si>
+  <si>
+    <t>my candidacy</t>
+  </si>
+  <si>
+    <t>sometimes complex</t>
   </si>
 </sst>
 </file>
@@ -276,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -287,6 +300,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -589,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L20"/>
+  <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -604,406 +629,444 @@
     <col min="5" max="5" width="1" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="37.5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="6" customHeight="1"/>
-    <row r="2" spans="2:12" ht="72">
+    <row r="2" spans="2:12" ht="54">
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
+      <c r="H2" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="3">
+        <v>3</v>
+      </c>
+      <c r="H3" s="10">
         <v>6</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="3">
+        <v>4</v>
+      </c>
+      <c r="H4" s="10">
         <v>7</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:12">
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>49</v>
+        <v>3</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="10">
         <v>6</v>
       </c>
-      <c r="H6" s="3">
-        <v>6</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="36">
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="2:12" ht="6" customHeight="1">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="2:12" ht="36.75" customHeight="1">
-      <c r="B9" s="3" t="s">
+      <c r="F7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="10">
+        <v>4</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="L7" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="3">
-        <v>8</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="3">
-        <v>7</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="2:12" ht="6" customHeight="1">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="F11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="36.75" customHeight="1">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12">
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
+      <c r="D12" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="10">
+        <v>8</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="L12" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="54">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="3">
-        <v>4</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="10"/>
       <c r="I13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D14" s="3" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3">
-        <v>4</v>
-      </c>
-      <c r="I14" s="3"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="J14" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="H15" s="10"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="10">
+        <v>4</v>
+      </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="20" spans="5:10">
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="L16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>